<commit_message>
Them cot nhiem vu cho tab gtn
</commit_message>
<xml_diff>
--- a/Final_Project/DSTV.xlsx
+++ b/Final_Project/DSTV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\3rd_Year\First_term\PPT_Matlab\Theory_PPT_Matlab\Matlab\PPT\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5183DD39-D124-4203-9E37-5038E8701BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04157991-681C-40F5-8F8F-E4C90CB961E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Võ Thành Danh</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>Lê Minh Thành</t>
+  </si>
+  <si>
+    <t>Tab Tìm nghiệm</t>
+  </si>
+  <si>
+    <t>Tab Nội suy</t>
+  </si>
+  <si>
+    <t>Tab Hồi quy + Giới thiệu nhóm</t>
+  </si>
+  <si>
+    <t>Tab Đạo hàm</t>
+  </si>
+  <si>
+    <t>Tab Tích phân</t>
   </si>
 </sst>
 </file>
@@ -360,19 +375,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:U26"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -382,8 +398,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -393,8 +412,11 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -404,8 +426,11 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -415,8 +440,11 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -426,8 +454,11 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -436,6 +467,9 @@
       </c>
       <c r="C6" t="s">
         <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chinh lai tab gtn va do thi tab tim nghiem
</commit_message>
<xml_diff>
--- a/Final_Project/DSTV.xlsx
+++ b/Final_Project/DSTV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\3rd_Year\First_term\PPT_Matlab\Theory_PPT_Matlab\Matlab\PPT\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04157991-681C-40F5-8F8F-E4C90CB961E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57AB852-8B4C-494B-B96B-49BAB667898C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2916" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Võ Thành Danh</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Trần Tuấn Kiệt</t>
   </si>
   <si>
-    <t>Phan Hữu Phước</t>
-  </si>
-  <si>
     <t>Lê Đoàn Phú Sang</t>
   </si>
   <si>
@@ -51,13 +48,19 @@
     <t>Tab Nội suy</t>
   </si>
   <si>
-    <t>Tab Hồi quy + Giới thiệu nhóm</t>
-  </si>
-  <si>
     <t>Tab Đạo hàm</t>
   </si>
   <si>
     <t>Tab Tích phân</t>
+  </si>
+  <si>
+    <t>Phan Hữu Phước (Trưởng nhóm)</t>
+  </si>
+  <si>
+    <t>Tab Tìm nghiệm + Giới thiệu nhóm</t>
+  </si>
+  <si>
+    <t>Tab Hồi quy</t>
   </si>
 </sst>
 </file>
@@ -378,14 +381,14 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -393,10 +396,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>21200275</v>
+        <v>21200333</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -407,10 +410,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>21200278</v>
+        <v>21200275</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -421,13 +424,13 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>21200304</v>
+        <v>21200278</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -435,13 +438,13 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>21200333</v>
+        <v>21200304</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -452,10 +455,10 @@
         <v>21200346</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -466,10 +469,10 @@
         <v>21200351</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>